<commit_message>
add postal code column
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Apiary_Sites_Template.xlsx
+++ b/app/server/static/templates/reports/Apiary_Sites_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikeg\Desktop\work\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AAC5CD-B142-4F78-B0C5-A7B0A160F06A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203FBAF7-A2D2-4EF1-8B0E-CA5224654359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="23085" windowHeight="15030" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Apiary Producer" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Last Name</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>{d.Reg[i].LastName}</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>{d.Reg[i].Postal_Code}</t>
   </si>
 </sst>
 </file>
@@ -182,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -197,26 +203,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -544,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,49 +553,47 @@
     <col min="8" max="8" width="19.28515625" customWidth="1"/>
     <col min="9" max="9" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1"/>
     <col min="13" max="13" width="15.7109375" customWidth="1"/>
     <col min="18" max="19" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="12"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="12"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
@@ -620,16 +611,16 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C5" s="6"/>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -653,7 +644,7 @@
       <c r="G6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I6" s="5" t="s">
@@ -662,13 +653,15 @@
       <c r="J6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
@@ -678,68 +671,71 @@
       <c r="T6" s="5"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="K7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="M7" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="11"/>
+      <c r="C8" s="8"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="9"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K13" s="7"/>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K14" s="7"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K15" s="7"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="17" t="s">
+      <c r="J22" s="12" t="s">
         <v>8</v>
       </c>
       <c r="K22" s="4" t="s">
@@ -756,18 +752,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -982,6 +978,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03155FF8-1FF1-4181-B2B9-505B2808F58D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AE8867F-A406-43FE-8CA7-900664EF104F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -994,14 +998,6 @@
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
     <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03155FF8-1FF1-4181-B2B9-505B2808F58D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
add site id to apiary site template
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Apiary_Sites_Template.xlsx
+++ b/app/server/static/templates/reports/Apiary_Sites_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikeg\Desktop\work\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AAC5CD-B142-4F78-B0C5-A7B0A160F06A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC58C20E-D3AC-4437-A972-54213C72B75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="3510" yWindow="3345" windowWidth="23085" windowHeight="15030" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Apiary Producer" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Last Name</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>{d.Reg[i].LastName}</t>
+  </si>
+  <si>
+    <t>Site ID</t>
+  </si>
+  <si>
+    <t>{d.Reg[i].SiteId}</t>
   </si>
 </sst>
 </file>
@@ -182,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -197,26 +203,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -227,6 +220,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,14 +541,14 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
@@ -567,42 +563,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="12"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="12"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
       <c r="K2" s="1"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
@@ -620,16 +615,16 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C5" s="6"/>
-      <c r="D5" s="18" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -638,37 +633,39 @@
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
@@ -678,71 +675,74 @@
       <c r="T6" s="5"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="I7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="J7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="K7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="L7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="M7" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="11"/>
+      <c r="C8" s="8"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="9"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K13" s="7"/>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K14" s="7"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K15" s="7"/>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="17" t="s">
+      <c r="K15" s="6"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C22" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="17" t="s">
+      <c r="K22" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="L22" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -756,18 +756,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -982,6 +982,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03155FF8-1FF1-4181-B2B9-505B2808F58D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AE8867F-A406-43FE-8CA7-900664EF104F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -994,14 +1002,6 @@
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
     <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03155FF8-1FF1-4181-B2B9-505B2808F58D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>